<commit_message>
Update with more certificates
git-svn-id: https://svn.softwareboersen.dk/openebusiness/dk.gov.oiosi/library/dotnet/trunk@18817 4e58de57-8926-0410-947e-8945c843cdd7
</commit_message>
<xml_diff>
--- a/src/dk.gov.oiosi.resource/Resources/Certificates/Certifikate.xlsx
+++ b/src/dk.gov.oiosi.resource/Resources/Certificates/Certifikate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="54">
   <si>
     <t>Udløber</t>
   </si>
@@ -133,6 +133,51 @@
   </si>
   <si>
     <t>.\Live\Funktionscertifikat\CVR26769388.Expire20120104.NemHandel test service.cer</t>
+  </si>
+  <si>
+    <t>Medarbejderscertifikat</t>
+  </si>
+  <si>
+    <t>.\Test\Funktionscertifikat\CVR30808460.Expire20091126.Test MOCES1 (medarbejdercertificat 3)(Expired).pfx</t>
+  </si>
+  <si>
+    <t>MedarbejderCertifikat</t>
+  </si>
+  <si>
+    <t>26-011-2009</t>
+  </si>
+  <si>
+    <t>‎40 37 66 be</t>
+  </si>
+  <si>
+    <t>SERIALNUMBER = CVR:30808460-RID:1259070771320</t>
+  </si>
+  <si>
+    <t>CN = Test MOCES3 (Expired)</t>
+  </si>
+  <si>
+    <t>.\Test\Funktionscertifikat\CVR30808460.Expire20130307.Test MOCES1 (medarbejdercertificat 1).pfx</t>
+  </si>
+  <si>
+    <t>‎40 37 c9 44</t>
+  </si>
+  <si>
+    <t>SERIALNUMBER = CVR:30808460-RID:1237553529373</t>
+  </si>
+  <si>
+    <t>CN = Test MOCES1</t>
+  </si>
+  <si>
+    <t>‎40 37 c9 48</t>
+  </si>
+  <si>
+    <t>SERIALNUMBER = CVR:30808460-RID:1237553579579</t>
+  </si>
+  <si>
+    <t>CN = Test MOCES2</t>
+  </si>
+  <si>
+    <t>.\Test\Funktionscertifikat\CVR30808460.Expire20130307.Test MOCES1 (medarbejdercertificat 2)(Spærret).pfx</t>
   </si>
 </sst>
 </file>
@@ -507,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E94"/>
+  <dimension ref="A2:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F127" sqref="F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1060,6 +1105,245 @@
         <v>21</v>
       </c>
       <c r="E94" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="15.75">
+      <c r="B97" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5">
+      <c r="C98" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5">
+      <c r="D99" t="s">
+        <v>24</v>
+      </c>
+      <c r="E99" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5">
+      <c r="E100" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5">
+      <c r="E101" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5">
+      <c r="D102" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5">
+      <c r="D103" t="s">
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5">
+      <c r="D104" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5">
+      <c r="D105" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5">
+      <c r="E106" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5">
+      <c r="E107" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5">
+      <c r="E108" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5">
+      <c r="D109" t="s">
+        <v>21</v>
+      </c>
+      <c r="E109" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5">
+      <c r="C111" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5">
+      <c r="D112" t="s">
+        <v>24</v>
+      </c>
+      <c r="E112" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="113" spans="3:5">
+      <c r="E113" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114" spans="3:5">
+      <c r="E114" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" spans="3:5">
+      <c r="D115" t="s">
+        <v>0</v>
+      </c>
+      <c r="E115" s="1">
+        <v>41340</v>
+      </c>
+    </row>
+    <row r="116" spans="3:5">
+      <c r="D116" t="s">
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="3:5">
+      <c r="D117" t="s">
+        <v>5</v>
+      </c>
+      <c r="E117" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="118" spans="3:5">
+      <c r="D118" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="119" spans="3:5">
+      <c r="E119" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="120" spans="3:5">
+      <c r="E120" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="3:5">
+      <c r="E121" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="3:5">
+      <c r="D122" t="s">
+        <v>21</v>
+      </c>
+      <c r="E122" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124" spans="3:5">
+      <c r="C124" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="125" spans="3:5">
+      <c r="D125" t="s">
+        <v>24</v>
+      </c>
+      <c r="E125" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="126" spans="3:5">
+      <c r="E126" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="127" spans="3:5">
+      <c r="E127" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="128" spans="3:5">
+      <c r="D128" t="s">
+        <v>0</v>
+      </c>
+      <c r="E128" s="1">
+        <v>41340</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5">
+      <c r="D129" t="s">
+        <v>1</v>
+      </c>
+      <c r="E129" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5">
+      <c r="D130" t="s">
+        <v>5</v>
+      </c>
+      <c r="E130" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5">
+      <c r="D131" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5">
+      <c r="E132" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5">
+      <c r="E133" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5">
+      <c r="E134" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5">
+      <c r="D135" t="s">
+        <v>21</v>
+      </c>
+      <c r="E135" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bug 579 - opdateret test koden. Rettet fejlen, så der kun bliver sendt til endpoint der også accepter den profil som dokumentet indeholder.
git-svn-id: https://svn.softwareboersen.dk/openebusiness/dk.gov.oiosi/library/dotnet/trunk@18832 4e58de57-8926-0410-947e-8945c843cdd7
</commit_message>
<xml_diff>
--- a/src/dk.gov.oiosi.resource/Resources/Certificates/Certifikate.xlsx
+++ b/src/dk.gov.oiosi.resource/Resources/Certificates/Certifikate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="63">
   <si>
     <t>Udløber</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Medarbejderscertifikat</t>
   </si>
   <si>
-    <t>.\Test\Funktionscertifikat\CVR30808460.Expire20091126.Test MOCES1 (medarbejdercertificat 3)(Expired).pfx</t>
-  </si>
-  <si>
     <t>MedarbejderCertifikat</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>CN = Test MOCES3 (Expired)</t>
   </si>
   <si>
-    <t>.\Test\Funktionscertifikat\CVR30808460.Expire20130307.Test MOCES1 (medarbejdercertificat 1).pfx</t>
-  </si>
-  <si>
     <t>‎40 37 c9 44</t>
   </si>
   <si>
@@ -177,7 +171,40 @@
     <t>CN = Test MOCES2</t>
   </si>
   <si>
-    <t>.\Test\Funktionscertifikat\CVR30808460.Expire20130307.Test MOCES1 (medarbejdercertificat 2)(Spærret).pfx</t>
+    <t>.\Test\Funktionscertifikat\CVR26769388.Expire20100417.Testendpoint.pfx</t>
+  </si>
+  <si>
+    <t>.\Test\Funktionscertifikat\CVR26769388.Expire20120427.Test NemHandelservice.pfx</t>
+  </si>
+  <si>
+    <t>.\Test\Medarbejdercertifikat\CVR30808460.Expire20130307.Test MOCES1 (medarbejdercertificat 2)(Spærret).pfx</t>
+  </si>
+  <si>
+    <t>.\Test\Medarbejdercertifikat\CVR30808460.Expire20130307.Test MOCES1 (medarbejdercertificat 1).pfx</t>
+  </si>
+  <si>
+    <t>.\Test\Medarbejdercertifikat\CVR30808460.Expire20091126.Test MOCES1 (medarbejdercertificat 3)(Expired).pfx</t>
+  </si>
+  <si>
+    <t>CN = Testendpoint (funktionscertifikat)</t>
+  </si>
+  <si>
+    <t>SERIALNUMBER = CVR:26769388-FID:1208430425605</t>
+  </si>
+  <si>
+    <t>CVR:26769388</t>
+  </si>
+  <si>
+    <t>‎40 36 d8 5e</t>
+  </si>
+  <si>
+    <t>CN = Test NemHandelservice (funktionscertifikat)</t>
+  </si>
+  <si>
+    <t>SERIALNUMBER = CVR:26769388-FID:1272375084431</t>
+  </si>
+  <si>
+    <t>‎40 37 81 63</t>
   </si>
 </sst>
 </file>
@@ -250,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -258,6 +285,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E135"/>
+  <dimension ref="A2:G148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F127" sqref="F127"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -836,12 +865,12 @@
         <v>50211</v>
       </c>
     </row>
-    <row r="49" spans="2:5">
+    <row r="49" spans="2:7">
       <c r="D49" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:5">
+    <row r="50" spans="2:7">
       <c r="D50" t="s">
         <v>5</v>
       </c>
@@ -849,193 +878,247 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:5">
+    <row r="51" spans="2:7">
       <c r="D51" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="2:7">
       <c r="E52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" spans="2:7">
       <c r="E53" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="2:5">
+    <row r="54" spans="2:7">
       <c r="E54" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="15.75">
+    <row r="56" spans="2:7" ht="15.75">
       <c r="B56" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="2:5">
+    <row r="57" spans="2:7">
       <c r="C57" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5">
-      <c r="D58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="D58" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="59" spans="2:5">
-      <c r="E59" t="s">
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="2:7">
+      <c r="D59" s="7"/>
+      <c r="E59" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="60" spans="2:5">
-      <c r="E60" t="s">
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="2:7">
+      <c r="D60" s="7"/>
+      <c r="E60" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="2:5">
-      <c r="D61" t="s">
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="2:7">
+      <c r="D61" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E61" s="1">
-        <v>41340</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5">
-      <c r="D62" t="s">
+      <c r="E61" s="8">
+        <v>40285</v>
+      </c>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="2:7">
+      <c r="D62" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="2:5">
-      <c r="D63" t="s">
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="2:7">
+      <c r="D63" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E63" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5">
-      <c r="D64" t="s">
+      <c r="E63" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64" spans="2:7">
+      <c r="D64" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E64" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="3:5">
-      <c r="E65" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="3:5">
-      <c r="E66" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="3:5">
-      <c r="E67" t="s">
+      <c r="E64" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="3:7">
+      <c r="D65" s="7"/>
+      <c r="E65" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+    </row>
+    <row r="66" spans="3:7">
+      <c r="D66" s="7"/>
+      <c r="E66" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+    </row>
+    <row r="67" spans="3:7">
+      <c r="D67" s="7"/>
+      <c r="E67" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="3:5">
-      <c r="D68" t="s">
-        <v>21</v>
-      </c>
-      <c r="E68" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="70" spans="3:5">
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+    </row>
+    <row r="68" spans="3:7">
+      <c r="D68" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+    </row>
+    <row r="70" spans="3:7">
       <c r="C70" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7">
+      <c r="D71" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+    </row>
+    <row r="72" spans="3:7">
+      <c r="D72" s="7"/>
+      <c r="E72" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+    </row>
+    <row r="73" spans="3:7">
+      <c r="D73" s="7"/>
+      <c r="E73" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+    </row>
+    <row r="74" spans="3:7">
+      <c r="D74" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="8">
+        <v>41026</v>
+      </c>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+    </row>
+    <row r="75" spans="3:7">
+      <c r="D75" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" spans="3:7">
+      <c r="D76" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+    </row>
+    <row r="77" spans="3:7">
+      <c r="D77" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+    </row>
+    <row r="78" spans="3:7">
+      <c r="D78" s="7"/>
+      <c r="E78" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+    </row>
+    <row r="79" spans="3:7">
+      <c r="D79" s="7"/>
+      <c r="E79" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+    </row>
+    <row r="80" spans="3:7">
+      <c r="D80" s="7"/>
+      <c r="E80" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+    </row>
+    <row r="81" spans="3:7">
+      <c r="D81" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+    </row>
+    <row r="83" spans="3:7">
+      <c r="C83" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="3:5">
-      <c r="D71" t="s">
-        <v>24</v>
-      </c>
-      <c r="E71" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="72" spans="3:5">
-      <c r="E72" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="3:5">
-      <c r="E73" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" spans="3:5">
-      <c r="D74" t="s">
-        <v>0</v>
-      </c>
-      <c r="E74" s="1">
-        <v>40832</v>
-      </c>
-    </row>
-    <row r="75" spans="3:5">
-      <c r="D75" t="s">
-        <v>1</v>
-      </c>
-      <c r="E75" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="3:5">
-      <c r="D76" t="s">
-        <v>5</v>
-      </c>
-      <c r="E76" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="3:5">
-      <c r="D77" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="3:5">
-      <c r="E78" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="3:5">
-      <c r="E79" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" spans="3:5">
-      <c r="E80" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="81" spans="3:5">
-      <c r="D81" t="s">
-        <v>21</v>
-      </c>
-      <c r="E81" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="83" spans="3:5">
-      <c r="C83" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="3:5">
+    <row r="84" spans="3:7">
       <c r="D84" t="s">
         <v>24</v>
       </c>
@@ -1043,25 +1126,25 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="3:5">
+    <row r="85" spans="3:7">
       <c r="E85" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="3:5">
+    <row r="86" spans="3:7">
       <c r="E86" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="3:5">
+    <row r="87" spans="3:7">
       <c r="D87" t="s">
         <v>0</v>
       </c>
       <c r="E87" s="1">
-        <v>41340</v>
-      </c>
-    </row>
-    <row r="88" spans="3:5">
+        <v>40832</v>
+      </c>
+    </row>
+    <row r="88" spans="3:7">
       <c r="D88" t="s">
         <v>1</v>
       </c>
@@ -1069,15 +1152,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="3:5">
+    <row r="89" spans="3:7">
       <c r="D89" t="s">
         <v>5</v>
       </c>
       <c r="E89" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="90" spans="3:5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="3:7">
       <c r="D90" t="s">
         <v>8</v>
       </c>
@@ -1085,22 +1168,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="3:5">
+    <row r="91" spans="3:7">
       <c r="E91" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="3:5">
+    <row r="92" spans="3:7">
       <c r="E92" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="3:5">
+    <row r="93" spans="3:7">
       <c r="E93" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="3:5">
+    <row r="94" spans="3:7">
       <c r="D94" t="s">
         <v>21</v>
       </c>
@@ -1108,92 +1191,92 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="2:5" ht="15.75">
-      <c r="B97" s="5" t="s">
-        <v>39</v>
+    <row r="96" spans="3:7">
+      <c r="C96" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5">
+      <c r="D97" t="s">
+        <v>24</v>
+      </c>
+      <c r="E97" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="2:5">
-      <c r="C98" s="4" t="s">
-        <v>40</v>
+      <c r="E98" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="2:5">
-      <c r="D99" t="s">
-        <v>24</v>
-      </c>
       <c r="E99" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="2:5">
-      <c r="E100" t="s">
-        <v>28</v>
+      <c r="D100" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="1">
+        <v>41340</v>
       </c>
     </row>
     <row r="101" spans="2:5">
+      <c r="D101" t="s">
+        <v>1</v>
+      </c>
       <c r="E101" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="2:5">
       <c r="D102" t="s">
-        <v>0</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>42</v>
+        <v>5</v>
+      </c>
+      <c r="E102" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="2:5">
       <c r="D103" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E103" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="2:5">
-      <c r="D104" t="s">
-        <v>5</v>
-      </c>
       <c r="E104" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="2:5">
-      <c r="D105" t="s">
-        <v>8</v>
-      </c>
       <c r="E105" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="2:5">
       <c r="E106" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="2:5">
+      <c r="D107" t="s">
+        <v>21</v>
+      </c>
       <c r="E107" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5">
-      <c r="E108" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="109" spans="2:5">
-      <c r="D109" t="s">
-        <v>21</v>
-      </c>
-      <c r="E109" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" ht="15.75">
+      <c r="B110" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="111" spans="2:5">
       <c r="C111" s="4" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="112" spans="2:5">
@@ -1201,7 +1284,7 @@
         <v>24</v>
       </c>
       <c r="E112" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="113" spans="3:5">
@@ -1218,8 +1301,8 @@
       <c r="D115" t="s">
         <v>0</v>
       </c>
-      <c r="E115" s="1">
-        <v>41340</v>
+      <c r="E115" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="116" spans="3:5">
@@ -1235,7 +1318,7 @@
         <v>5</v>
       </c>
       <c r="E117" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="118" spans="3:5">
@@ -1243,12 +1326,12 @@
         <v>8</v>
       </c>
       <c r="E118" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="119" spans="3:5">
       <c r="E119" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="120" spans="3:5">
@@ -1271,7 +1354,7 @@
     </row>
     <row r="124" spans="3:5">
       <c r="C124" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="125" spans="3:5">
@@ -1279,7 +1362,7 @@
         <v>24</v>
       </c>
       <c r="E125" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="126" spans="3:5">
@@ -1300,7 +1383,7 @@
         <v>41340</v>
       </c>
     </row>
-    <row r="129" spans="4:5">
+    <row r="129" spans="3:6">
       <c r="D129" t="s">
         <v>1</v>
       </c>
@@ -1308,42 +1391,121 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="4:5">
+    <row r="130" spans="3:6">
       <c r="D130" t="s">
         <v>5</v>
       </c>
       <c r="E130" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="131" spans="4:5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="131" spans="3:6">
       <c r="D131" t="s">
         <v>8</v>
       </c>
       <c r="E131" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="132" spans="4:5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="132" spans="3:6">
       <c r="E132" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="133" spans="4:5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="133" spans="3:6">
       <c r="E133" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="4:5">
+    <row r="134" spans="3:6">
       <c r="E134" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="4:5">
+    <row r="135" spans="3:6">
       <c r="D135" t="s">
         <v>21</v>
       </c>
       <c r="E135" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="137" spans="3:6">
+      <c r="C137" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="138" spans="3:6">
+      <c r="D138" t="s">
+        <v>24</v>
+      </c>
+      <c r="E138" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="139" spans="3:6">
+      <c r="E139" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="140" spans="3:6">
+      <c r="E140" t="s">
+        <v>23</v>
+      </c>
+      <c r="F140" s="4"/>
+    </row>
+    <row r="141" spans="3:6">
+      <c r="D141" t="s">
+        <v>0</v>
+      </c>
+      <c r="E141" s="1">
+        <v>41340</v>
+      </c>
+    </row>
+    <row r="142" spans="3:6">
+      <c r="D142" t="s">
+        <v>1</v>
+      </c>
+      <c r="E142" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="3:6">
+      <c r="D143" t="s">
+        <v>5</v>
+      </c>
+      <c r="E143" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="144" spans="3:6">
+      <c r="D144" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="145" spans="4:5">
+      <c r="E145" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="146" spans="4:5">
+      <c r="E146" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="4:5">
+      <c r="E147" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="148" spans="4:5">
+      <c r="D148" t="s">
+        <v>21</v>
+      </c>
+      <c r="E148" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>